<commit_message>
eddy ni 1999-2000 (update 2)
</commit_message>
<xml_diff>
--- a/_data/ni/ni9900/individueel_eindstand_dworp_123_9900.xlsx
+++ b/_data/ni/ni9900/individueel_eindstand_dworp_123_9900.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="14520" windowHeight="12840"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="14520" windowHeight="12840" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1367" uniqueCount="236">
   <si>
     <t>Jaar 1</t>
   </si>
@@ -185,9 +185,6 @@
   </si>
   <si>
     <t>ng</t>
-  </si>
-  <si>
-    <t>(bye)</t>
   </si>
   <si>
     <t>bron: het blauwe jaarverslag 1999-2000 van Pieter Ertveldt.</t>
@@ -1833,7 +1830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
@@ -1887,10 +1884,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="69" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D7" s="69"/>
     </row>
@@ -1902,7 +1899,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="D11" s="69" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E11" s="69"/>
       <c r="F11" s="69"/>
@@ -1912,7 +1909,7 @@
     </row>
     <row r="21" spans="4:20">
       <c r="D21" s="69" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E21" s="69"/>
       <c r="F21" s="69"/>
@@ -1933,7 +1930,7 @@
     </row>
     <row r="22" spans="4:20">
       <c r="D22" s="69" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E22" s="69"/>
       <c r="F22" s="69"/>
@@ -1954,7 +1951,7 @@
     </row>
     <row r="23" spans="4:20">
       <c r="D23" s="69" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E23" s="69"/>
       <c r="F23" s="69"/>
@@ -1975,7 +1972,7 @@
     </row>
     <row r="24" spans="4:20">
       <c r="D24" s="68" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E24" s="68"/>
       <c r="F24" s="68"/>
@@ -1997,7 +1994,7 @@
     <row r="25" spans="4:20">
       <c r="D25" s="68"/>
       <c r="E25" s="68" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F25" s="68"/>
       <c r="G25" s="68"/>
@@ -2017,7 +2014,7 @@
     </row>
     <row r="26" spans="4:20">
       <c r="D26" s="69" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E26" s="69"/>
       <c r="F26" s="69"/>
@@ -2038,7 +2035,7 @@
     </row>
     <row r="27" spans="4:20">
       <c r="D27" s="68" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E27" s="68"/>
       <c r="F27" s="68"/>
@@ -2059,7 +2056,7 @@
     </row>
     <row r="28" spans="4:20">
       <c r="D28" s="68" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E28" s="68"/>
       <c r="F28" s="68"/>
@@ -2080,7 +2077,7 @@
     </row>
     <row r="29" spans="4:20">
       <c r="D29" s="69" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E29" s="69"/>
       <c r="F29" s="69"/>
@@ -2137,7 +2134,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -2151,7 +2148,7 @@
       </c>
       <c r="J3" s="1"/>
       <c r="L3" s="68" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -2192,7 +2189,7 @@
         <v>69639</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D5" s="18">
         <v>1919</v>
@@ -2210,7 +2207,7 @@
         <v>2283</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J5" s="18">
         <v>1961</v>
@@ -2224,7 +2221,7 @@
         <v>50016</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D6" s="18">
         <v>1760</v>
@@ -2256,7 +2253,7 @@
         <v>79618</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D7" s="18">
         <v>1706</v>
@@ -2288,7 +2285,7 @@
         <v>71269</v>
       </c>
       <c r="C8" s="70" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D8" s="18">
         <v>1683</v>
@@ -2306,7 +2303,7 @@
         <v>2259</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J8" s="18">
         <v>1234</v>
@@ -2379,7 +2376,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -2393,7 +2390,7 @@
       </c>
       <c r="J13" s="1"/>
       <c r="L13" s="68" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -2434,7 +2431,7 @@
         <v>17906</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D15" s="18">
         <v>1830</v>
@@ -2452,7 +2449,7 @@
         <v>76325</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J15" s="18">
         <v>1845</v>
@@ -2466,7 +2463,7 @@
         <v>79689</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D16" s="18">
         <v>1808</v>
@@ -2498,7 +2495,7 @@
         <v>80918</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D17" s="18">
         <v>1795</v>
@@ -2530,7 +2527,7 @@
         <v>52094</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D18" s="18">
         <v>1754</v>
@@ -2548,7 +2545,7 @@
         <v>54658</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J18" s="18">
         <v>1452</v>
@@ -2589,7 +2586,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -2603,7 +2600,7 @@
       </c>
       <c r="J21" s="1"/>
       <c r="L21" s="68" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -2644,7 +2641,7 @@
         <v>89401</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D23" s="18">
         <v>1524</v>
@@ -2676,7 +2673,7 @@
         <v>84603</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D24" s="18">
         <v>1514</v>
@@ -2708,7 +2705,7 @@
         <v>59668</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D25" s="18">
         <v>1410</v>
@@ -2740,7 +2737,7 @@
         <v>74802</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D26" s="18">
         <v>1365</v>
@@ -2758,7 +2755,7 @@
         <v>48097</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J26" s="18" t="s">
         <v>52</v>
@@ -2984,7 +2981,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -3026,7 +3023,7 @@
         <v>2283</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" s="18">
         <v>1961</v>
@@ -3044,7 +3041,7 @@
         <v>9814</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J5" s="18">
         <v>1977</v>
@@ -3076,7 +3073,7 @@
         <v>40142</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J6" s="18">
         <v>1973</v>
@@ -3108,13 +3105,13 @@
         <v>11169</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J7" s="18">
         <v>1973</v>
       </c>
       <c r="L7" s="68" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M7" s="68"/>
       <c r="N7" s="68"/>
@@ -3127,7 +3124,7 @@
         <v>2259</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8" s="18">
         <v>1234</v>
@@ -3145,13 +3142,13 @@
         <v>43613</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J8" s="18">
         <v>1894</v>
       </c>
       <c r="L8" s="68" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M8" s="68"/>
       <c r="N8" s="68"/>
@@ -3233,7 +3230,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -3273,7 +3270,7 @@
       </c>
       <c r="B15" s="19"/>
       <c r="C15" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="10">
@@ -3287,7 +3284,7 @@
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J15" s="18"/>
     </row>
@@ -3297,7 +3294,7 @@
       </c>
       <c r="B16" s="19"/>
       <c r="C16" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="10">
@@ -3311,7 +3308,7 @@
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J16" s="18"/>
     </row>
@@ -3341,7 +3338,7 @@
         <v>74543</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J17" s="18">
         <v>1414</v>
@@ -3355,7 +3352,7 @@
         <v>54658</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D18" s="18">
         <v>1452</v>
@@ -3373,7 +3370,7 @@
         <v>94901</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J18" s="18">
         <v>1340</v>
@@ -3424,7 +3421,7 @@
         <v>12</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -3484,13 +3481,13 @@
         <v>21733</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J23" s="18">
         <v>1894</v>
       </c>
       <c r="L23" s="68" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M23" s="68"/>
       <c r="N23" s="68"/>
@@ -3523,7 +3520,7 @@
         <v>51578</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J24" s="18">
         <v>1584</v>
@@ -3555,7 +3552,7 @@
         <v>52736</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J25" s="18" t="s">
         <v>52</v>
@@ -3569,7 +3566,7 @@
         <v>48097</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>52</v>
@@ -3587,7 +3584,7 @@
         <v>25879</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J26" s="18" t="s">
         <v>52</v>
@@ -3803,7 +3800,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -3855,7 +3852,7 @@
         <v>56294</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D5" s="18">
         <v>1927</v>
@@ -3873,7 +3870,7 @@
         <v>2283</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J5" s="18">
         <v>1961</v>
@@ -3887,7 +3884,7 @@
         <v>80616</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D6" s="18">
         <v>1907</v>
@@ -3919,7 +3916,7 @@
         <v>46281</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D7" s="18">
         <v>1873</v>
@@ -3951,7 +3948,7 @@
         <v>14133</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D8" s="18">
         <v>1669</v>
@@ -3969,7 +3966,7 @@
         <v>54658</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J8" s="18">
         <v>1452</v>
@@ -4040,7 +4037,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -4092,7 +4089,7 @@
         <v>31739</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D15" s="18">
         <v>1694</v>
@@ -4110,7 +4107,7 @@
         <v>9954</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J15" s="18">
         <v>1831</v>
@@ -4124,7 +4121,7 @@
         <v>16365</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D16" s="18">
         <v>1613</v>
@@ -4142,7 +4139,7 @@
         <v>76325</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J16" s="18">
         <v>1845</v>
@@ -4156,7 +4153,7 @@
         <v>18538</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D17" s="18">
         <v>1662</v>
@@ -4188,7 +4185,7 @@
         <v>67164</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D18" s="18">
         <v>1602</v>
@@ -4206,7 +4203,7 @@
         <v>2259</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J18" s="18">
         <v>1234</v>
@@ -4247,7 +4244,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -4299,7 +4296,7 @@
         <v>92622</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D23" s="18">
         <v>1650</v>
@@ -4331,7 +4328,7 @@
         <v>33006</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D24" s="18">
         <v>1169</v>
@@ -4363,7 +4360,7 @@
         <v>81167</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D25" s="18">
         <v>1150</v>
@@ -4395,7 +4392,7 @@
         <v>80853</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D26" s="18">
         <v>1198</v>
@@ -4588,7 +4585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AQ280"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="R44" sqref="R44"/>
     </sheetView>
   </sheetViews>
@@ -4699,7 +4696,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C4" s="40" t="s">
         <v>37</v>
@@ -4850,7 +4847,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="39" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C5" s="41">
         <v>2</v>
@@ -5001,7 +4998,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C6" s="41">
         <v>0</v>
@@ -5152,7 +5149,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C7" s="41">
         <v>0.5</v>
@@ -5454,7 +5451,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="39" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C9" s="41">
         <v>0.5</v>
@@ -5605,7 +5602,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="39" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C10" s="41">
         <v>2.5</v>
@@ -5756,7 +5753,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C11" s="41">
         <v>0</v>
@@ -5907,7 +5904,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C12" s="41">
         <v>0.5</v>
@@ -6058,7 +6055,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="39" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C13" s="41">
         <v>1</v>
@@ -6209,7 +6206,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="39" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C14" s="41">
         <v>0</v>
@@ -6360,7 +6357,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="45" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C15" s="46">
         <v>0</v>
@@ -6605,7 +6602,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="39" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C18" s="40" t="s">
         <v>37</v>
@@ -6756,7 +6753,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="39" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C19" s="41">
         <v>1</v>
@@ -6907,7 +6904,7 @@
         <v>3</v>
       </c>
       <c r="B20" s="39" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C20" s="41">
         <v>1</v>
@@ -7058,7 +7055,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="39" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C21" s="41">
         <v>1.5</v>
@@ -7209,7 +7206,7 @@
         <v>5</v>
       </c>
       <c r="B22" s="39" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C22" s="41">
         <v>2</v>
@@ -7511,7 +7508,7 @@
         <v>7</v>
       </c>
       <c r="B24" s="39" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C24" s="41">
         <v>1</v>
@@ -7662,7 +7659,7 @@
         <v>8</v>
       </c>
       <c r="B25" s="39" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C25" s="41">
         <v>2</v>
@@ -7813,7 +7810,7 @@
         <v>9</v>
       </c>
       <c r="B26" s="39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C26" s="41">
         <v>1.5</v>
@@ -7964,7 +7961,7 @@
         <v>10</v>
       </c>
       <c r="B27" s="39" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C27" s="41">
         <v>1</v>
@@ -8115,7 +8112,7 @@
         <v>11</v>
       </c>
       <c r="B28" s="39" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C28" s="41">
         <v>1.5</v>
@@ -8266,7 +8263,7 @@
         <v>12</v>
       </c>
       <c r="B29" s="45" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C29" s="46">
         <v>2</v>
@@ -8548,7 +8545,7 @@
       </c>
       <c r="N32" s="41"/>
       <c r="O32" s="42">
-        <f t="shared" ref="O32:O43" si="31">SUM(C32:N32)</f>
+        <f t="shared" ref="O32:O42" si="31">SUM(C32:N32)</f>
         <v>31.5</v>
       </c>
       <c r="P32" s="42">
@@ -8556,7 +8553,7 @@
         <v>8.5</v>
       </c>
       <c r="Q32" s="43">
-        <f t="shared" ref="Q32:Q43" si="32">COUNT(C32:N32)</f>
+        <f t="shared" ref="Q32:Q42" si="32">COUNT(C32:N32)</f>
         <v>10</v>
       </c>
       <c r="R32" s="52"/>
@@ -8660,7 +8657,7 @@
         <v>2</v>
       </c>
       <c r="B33" s="39" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C33" s="41">
         <v>1</v>
@@ -8809,7 +8806,7 @@
         <v>3</v>
       </c>
       <c r="B34" s="39" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C34" s="41">
         <v>0</v>
@@ -8958,7 +8955,7 @@
         <v>4</v>
       </c>
       <c r="B35" s="39" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C35" s="41">
         <v>1.5</v>
@@ -9107,7 +9104,7 @@
         <v>5</v>
       </c>
       <c r="B36" s="39" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C36" s="41">
         <v>2.5</v>
@@ -9256,7 +9253,7 @@
         <v>6</v>
       </c>
       <c r="B37" s="39" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C37" s="41">
         <v>2</v>
@@ -9405,7 +9402,7 @@
         <v>7</v>
       </c>
       <c r="B38" s="39" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C38" s="41">
         <v>0</v>
@@ -9554,7 +9551,7 @@
         <v>8</v>
       </c>
       <c r="B39" s="39" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C39" s="41">
         <v>1.5</v>
@@ -9703,7 +9700,7 @@
         <v>9</v>
       </c>
       <c r="B40" s="39" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C40" s="41">
         <v>0</v>
@@ -9852,7 +9849,7 @@
         <v>10</v>
       </c>
       <c r="B41" s="39" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C41" s="41">
         <v>0</v>
@@ -10001,7 +9998,7 @@
         <v>11</v>
       </c>
       <c r="B42" s="39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C42" s="41">
         <v>0</v>
@@ -10149,9 +10146,7 @@
       <c r="A43" s="44">
         <v>12</v>
       </c>
-      <c r="B43" s="45" t="s">
-        <v>53</v>
-      </c>
+      <c r="B43" s="45"/>
       <c r="C43" s="46"/>
       <c r="D43" s="46"/>
       <c r="E43" s="46"/>
@@ -15065,7 +15060,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -15107,7 +15102,7 @@
         <v>2283</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" s="18">
         <v>1961</v>
@@ -15125,7 +15120,7 @@
         <v>5169</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J5" s="18">
         <v>1952</v>
@@ -15157,7 +15152,7 @@
         <v>20818</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J6" s="18">
         <v>1951</v>
@@ -15189,7 +15184,7 @@
         <v>32212</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J7" s="18">
         <v>1942</v>
@@ -15203,7 +15198,7 @@
         <v>43419</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" s="18">
         <v>1867</v>
@@ -15221,7 +15216,7 @@
         <v>20907</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J8" s="18">
         <v>1935</v>
@@ -15304,7 +15299,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -15346,7 +15341,7 @@
         <v>76325</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D15" s="18">
         <v>1845</v>
@@ -15364,7 +15359,7 @@
         <v>82848</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J15" s="18">
         <v>1743</v>
@@ -15396,7 +15391,7 @@
         <v>76937</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J16" s="18">
         <v>1672</v>
@@ -15428,7 +15423,7 @@
         <v>2941</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J17" s="18">
         <v>1607</v>
@@ -15460,7 +15455,7 @@
         <v>79201</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J18" s="18">
         <v>1546</v>
@@ -15511,7 +15506,7 @@
         <v>12</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -15571,7 +15566,7 @@
         <v>76236</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J23" s="18">
         <v>1392</v>
@@ -15585,7 +15580,7 @@
         <v>54658</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D24" s="18">
         <v>1452</v>
@@ -15603,7 +15598,7 @@
         <v>71439</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J24" s="18">
         <v>1375</v>
@@ -15617,7 +15612,7 @@
         <v>2259</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D25" s="18">
         <v>1234</v>
@@ -15635,7 +15630,7 @@
         <v>89729</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J25" s="18">
         <v>1275</v>
@@ -15649,7 +15644,7 @@
         <v>48097</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>52</v>
@@ -15667,7 +15662,7 @@
         <v>86916</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J26" s="18" t="s">
         <v>52</v>
@@ -15875,7 +15870,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -15927,7 +15922,7 @@
         <v>88781</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D5" s="18">
         <v>2016</v>
@@ -15945,7 +15940,7 @@
         <v>2283</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J5" s="18">
         <v>1961</v>
@@ -15959,7 +15954,7 @@
         <v>33405</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D6" s="18">
         <v>1865</v>
@@ -15991,7 +15986,7 @@
         <v>50504</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D7" s="18">
         <v>1715</v>
@@ -16023,7 +16018,7 @@
         <v>5088</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D8" s="18">
         <v>1714</v>
@@ -16114,7 +16109,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -16166,7 +16161,7 @@
         <v>24856</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D15" s="18">
         <v>1946</v>
@@ -16184,7 +16179,7 @@
         <v>9954</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J15" s="18">
         <v>1831</v>
@@ -16198,7 +16193,7 @@
         <v>41688</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D16" s="18">
         <v>1721</v>
@@ -16216,7 +16211,7 @@
         <v>76325</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J16" s="18">
         <v>1845</v>
@@ -16230,7 +16225,7 @@
         <v>9334</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D17" s="18">
         <v>1769</v>
@@ -16262,7 +16257,7 @@
         <v>12068</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D18" s="18">
         <v>1547</v>
@@ -16321,7 +16316,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -16373,7 +16368,7 @@
         <v>77828</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D23" s="18">
         <v>1529</v>
@@ -16405,7 +16400,7 @@
         <v>58025</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D24" s="18">
         <v>1554</v>
@@ -16437,7 +16432,7 @@
         <v>62511</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D25" s="18">
         <v>1528</v>
@@ -16455,7 +16450,7 @@
         <v>54658</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J25" s="18">
         <v>1452</v>
@@ -16469,7 +16464,7 @@
         <v>72842</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D26" s="18">
         <v>1251</v>
@@ -16487,7 +16482,7 @@
         <v>48097</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J26" s="18" t="s">
         <v>52</v>
@@ -16713,7 +16708,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -16755,7 +16750,7 @@
         <v>2283</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" s="18">
         <v>1961</v>
@@ -16773,7 +16768,7 @@
         <v>97063</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J5" s="18">
         <v>2131</v>
@@ -16805,7 +16800,7 @@
         <v>98671</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J6" s="18">
         <v>2012</v>
@@ -16837,7 +16832,7 @@
         <v>98451</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J7" s="18">
         <v>1849</v>
@@ -16851,7 +16846,7 @@
         <v>48097</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>52</v>
@@ -16869,7 +16864,7 @@
         <v>20931</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J8" s="18">
         <v>1690</v>
@@ -16952,7 +16947,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -16994,7 +16989,7 @@
         <v>9954</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D15" s="18">
         <v>1831</v>
@@ -17012,7 +17007,7 @@
         <v>48895</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J15" s="18">
         <v>1896</v>
@@ -17044,7 +17039,7 @@
         <v>99554</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J16" s="18">
         <v>1880</v>
@@ -17058,7 +17053,7 @@
         <v>76325</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D17" s="18">
         <v>1845</v>
@@ -17076,7 +17071,7 @@
         <v>99805</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J17" s="18">
         <v>1753</v>
@@ -17108,7 +17103,7 @@
         <v>15709</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J18" s="18">
         <v>1747</v>
@@ -17159,7 +17154,7 @@
         <v>12</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -17219,7 +17214,7 @@
         <v>45292</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J23" s="18">
         <v>1688</v>
@@ -17233,7 +17228,7 @@
         <v>54658</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D24" s="18">
         <v>1452</v>
@@ -17251,7 +17246,7 @@
         <v>3271</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J24" s="18">
         <v>1611</v>
@@ -17265,7 +17260,7 @@
         <v>2259</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D25" s="18">
         <v>1234</v>
@@ -17283,7 +17278,7 @@
         <v>27286</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J25" s="18">
         <v>1592</v>
@@ -17297,7 +17292,7 @@
         <v>41483</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>52</v>
@@ -17315,7 +17310,7 @@
         <v>26565</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J26" s="18">
         <v>1398</v>
@@ -17531,7 +17526,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -17583,7 +17578,7 @@
         <v>31399</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D5" s="18">
         <v>2094</v>
@@ -17601,7 +17596,7 @@
         <v>2283</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J5" s="18">
         <v>1961</v>
@@ -17615,7 +17610,7 @@
         <v>36447</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D6" s="18">
         <v>1849</v>
@@ -17647,7 +17642,7 @@
         <v>25313</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D7" s="18">
         <v>1675</v>
@@ -17679,7 +17674,7 @@
         <v>41858</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>52</v>
@@ -17697,7 +17692,7 @@
         <v>43419</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J8" s="18">
         <v>1867</v>
@@ -17770,7 +17765,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -17822,7 +17817,7 @@
         <v>66184</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D15" s="18">
         <v>2041</v>
@@ -17840,7 +17835,7 @@
         <v>9954</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J15" s="18">
         <v>1831</v>
@@ -17854,7 +17849,7 @@
         <v>81922</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D16" s="18">
         <v>1951</v>
@@ -17872,7 +17867,7 @@
         <v>76325</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J16" s="18">
         <v>1845</v>
@@ -17886,7 +17881,7 @@
         <v>87823</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D17" s="18">
         <v>1861</v>
@@ -17918,7 +17913,7 @@
         <v>36633</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D18" s="18">
         <v>1858</v>
@@ -17977,7 +17972,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -18027,7 +18022,7 @@
       </c>
       <c r="B23" s="19"/>
       <c r="C23" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="10">
@@ -18041,7 +18036,7 @@
       </c>
       <c r="H23" s="19"/>
       <c r="I23" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J23" s="18"/>
     </row>
@@ -18053,7 +18048,7 @@
         <v>61514</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D24" s="18">
         <v>1484</v>
@@ -18071,7 +18066,7 @@
         <v>54658</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J24" s="18">
         <v>1452</v>
@@ -18085,7 +18080,7 @@
         <v>54232</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D25" s="18">
         <v>1444</v>
@@ -18103,7 +18098,7 @@
         <v>2259</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J25" s="18">
         <v>1234</v>
@@ -18117,7 +18112,7 @@
         <v>90387</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D26" s="18">
         <v>1397</v>
@@ -18135,7 +18130,7 @@
         <v>48097</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J26" s="18" t="s">
         <v>52</v>
@@ -18349,7 +18344,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -18401,7 +18396,7 @@
         <v>87912</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D5" s="18">
         <v>2116</v>
@@ -18419,7 +18414,7 @@
         <v>2283</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J5" s="18">
         <v>1961</v>
@@ -18433,7 +18428,7 @@
         <v>2607</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D6" s="18">
         <v>2069</v>
@@ -18465,7 +18460,7 @@
         <v>37044</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D7" s="18">
         <v>1981</v>
@@ -18497,7 +18492,7 @@
         <v>2330</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D8" s="18">
         <v>1924</v>
@@ -18515,7 +18510,7 @@
         <v>43419</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J8" s="18">
         <v>1867</v>
@@ -18588,7 +18583,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -18640,7 +18635,7 @@
         <v>13731</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D15" s="18">
         <v>1847</v>
@@ -18658,7 +18653,7 @@
         <v>76325</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J15" s="18">
         <v>1845</v>
@@ -18672,7 +18667,7 @@
         <v>46361</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D16" s="18">
         <v>1844</v>
@@ -18704,7 +18699,7 @@
         <v>21636</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D17" s="18">
         <v>1768</v>
@@ -18736,7 +18731,7 @@
         <v>48691</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D18" s="18">
         <v>1653</v>
@@ -18795,7 +18790,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -18847,7 +18842,7 @@
         <v>84166</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D23" s="18">
         <v>1564</v>
@@ -18879,7 +18874,7 @@
         <v>80438</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>52</v>
@@ -18897,7 +18892,7 @@
         <v>54658</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J24" s="18">
         <v>1452</v>
@@ -18911,7 +18906,7 @@
         <v>91081</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>52</v>
@@ -18929,7 +18924,7 @@
         <v>2259</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J25" s="18">
         <v>1234</v>
@@ -18943,7 +18938,7 @@
         <v>89907</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>52</v>
@@ -18961,7 +18956,7 @@
         <v>48097</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J26" s="18" t="s">
         <v>52</v>
@@ -19187,7 +19182,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -19229,7 +19224,7 @@
         <v>2283</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" s="18">
         <v>1961</v>
@@ -19247,7 +19242,7 @@
         <v>34525</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J5" s="18">
         <v>2011</v>
@@ -19279,7 +19274,7 @@
         <v>49760</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J6" s="18">
         <v>1921</v>
@@ -19311,7 +19306,7 @@
         <v>13315</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J7" s="18">
         <v>1893</v>
@@ -19325,7 +19320,7 @@
         <v>48097</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>52</v>
@@ -19343,7 +19338,7 @@
         <v>2364</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J8" s="18">
         <v>1830</v>
@@ -19426,7 +19421,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -19466,7 +19461,7 @@
       </c>
       <c r="B15" s="19"/>
       <c r="C15" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="10">
@@ -19480,7 +19475,7 @@
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J15" s="18"/>
     </row>
@@ -19490,7 +19485,7 @@
       </c>
       <c r="B16" s="19"/>
       <c r="C16" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="10">
@@ -19504,7 +19499,7 @@
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J16" s="18"/>
     </row>
@@ -19534,7 +19529,7 @@
         <v>23281</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J17" s="18">
         <v>1869</v>
@@ -19564,7 +19559,7 @@
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J18" s="18"/>
     </row>
@@ -19613,7 +19608,7 @@
         <v>12</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -19653,7 +19648,7 @@
       </c>
       <c r="B23" s="19"/>
       <c r="C23" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="10">
@@ -19667,7 +19662,7 @@
       </c>
       <c r="H23" s="19"/>
       <c r="I23" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J23" s="18"/>
     </row>
@@ -19677,7 +19672,7 @@
       </c>
       <c r="B24" s="19"/>
       <c r="C24" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D24" s="18"/>
       <c r="E24" s="10">
@@ -19691,7 +19686,7 @@
       </c>
       <c r="H24" s="19"/>
       <c r="I24" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J24" s="18"/>
     </row>
@@ -19701,7 +19696,7 @@
       </c>
       <c r="B25" s="19"/>
       <c r="C25" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D25" s="18"/>
       <c r="E25" s="10">
@@ -19715,7 +19710,7 @@
       </c>
       <c r="H25" s="19"/>
       <c r="I25" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J25" s="18"/>
     </row>
@@ -19725,7 +19720,7 @@
       </c>
       <c r="B26" s="19"/>
       <c r="C26" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D26" s="18"/>
       <c r="E26" s="12">
@@ -19739,7 +19734,7 @@
       </c>
       <c r="H26" s="19"/>
       <c r="I26" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J26" s="18"/>
     </row>
@@ -19951,7 +19946,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -20001,7 +19996,7 @@
         <v>27413</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" s="18">
         <v>2050</v>
@@ -20019,7 +20014,7 @@
         <v>2283</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J5" s="18">
         <v>1961</v>
@@ -20033,7 +20028,7 @@
         <v>21113</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D6" s="18">
         <v>1888</v>
@@ -20065,7 +20060,7 @@
         <v>14605</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D7" s="18">
         <v>1886</v>
@@ -20097,7 +20092,7 @@
         <v>20664</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D8" s="18">
         <v>1814</v>
@@ -20115,7 +20110,7 @@
         <v>48097</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J8" s="18" t="s">
         <v>52</v>
@@ -20188,7 +20183,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -20238,7 +20233,7 @@
         <v>42307</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D15" s="18">
         <v>1922</v>
@@ -20256,7 +20251,7 @@
         <v>9954</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J15" s="18">
         <v>1831</v>
@@ -20270,7 +20265,7 @@
         <v>68497</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D16" s="18">
         <v>1865</v>
@@ -20302,7 +20297,7 @@
         <v>70017</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D17" s="18">
         <v>1737</v>
@@ -20320,13 +20315,13 @@
         <v>76325</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J17" s="18">
         <v>1845</v>
       </c>
       <c r="L17" s="68" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M17" s="68"/>
       <c r="N17" s="68"/>
@@ -20339,7 +20334,7 @@
         <v>66354</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D18" s="18">
         <v>1816</v>
@@ -20363,7 +20358,7 @@
         <v>1774</v>
       </c>
       <c r="L18" s="68" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M18" s="68"/>
       <c r="N18" s="68"/>
@@ -20403,7 +20398,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -20455,7 +20450,7 @@
         <v>90212</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D23" s="18">
         <v>1721</v>
@@ -20487,7 +20482,7 @@
         <v>70106</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D24" s="18">
         <v>1616</v>
@@ -20519,7 +20514,7 @@
         <v>69914</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D25" s="18">
         <v>1542</v>
@@ -20537,7 +20532,7 @@
         <v>54658</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J25" s="18">
         <v>1452</v>
@@ -20551,7 +20546,7 @@
         <v>77275</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D26" s="18">
         <v>1331</v>
@@ -20569,7 +20564,7 @@
         <v>2259</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J26" s="18">
         <v>1234</v>
@@ -20793,7 +20788,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -20835,7 +20830,7 @@
         <v>2283</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D5" s="18">
         <v>1961</v>
@@ -20853,7 +20848,7 @@
         <v>60330</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J5" s="18">
         <v>1871</v>
@@ -20885,7 +20880,7 @@
         <v>8044</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J6" s="18">
         <v>1744</v>
@@ -20917,7 +20912,7 @@
         <v>9229</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J7" s="18">
         <v>1709</v>
@@ -20949,7 +20944,7 @@
         <v>32000</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J8" s="18" t="s">
         <v>52</v>
@@ -21032,7 +21027,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -21074,7 +21069,7 @@
         <v>9954</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D15" s="18">
         <v>1831</v>
@@ -21092,7 +21087,7 @@
         <v>78549</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J15" s="18">
         <v>1523</v>
@@ -21124,7 +21119,7 @@
         <v>59579</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J16" s="18">
         <v>1516</v>
@@ -21138,7 +21133,7 @@
         <v>64327</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D17" s="18">
         <v>1552</v>
@@ -21156,7 +21151,7 @@
         <v>84476</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J17" s="18">
         <v>1279</v>
@@ -21170,7 +21165,7 @@
         <v>2259</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" s="18">
         <v>1234</v>
@@ -21188,7 +21183,7 @@
         <v>79696</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J18" s="18">
         <v>1164</v>
@@ -21239,7 +21234,7 @@
         <v>12</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J21" s="1"/>
     </row>
@@ -21281,7 +21276,7 @@
         <v>76325</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D23" s="18">
         <v>1845</v>
@@ -21299,7 +21294,7 @@
         <v>92452</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J23" s="18">
         <v>1896</v>
@@ -21331,7 +21326,7 @@
         <v>65722</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J24" s="18">
         <v>1855</v>
@@ -21363,7 +21358,7 @@
         <v>77615</v>
       </c>
       <c r="I25" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J25" s="18">
         <v>1918</v>
@@ -21377,7 +21372,7 @@
         <v>48097</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>52</v>
@@ -21395,7 +21390,7 @@
         <v>55760</v>
       </c>
       <c r="I26" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J26" s="18">
         <v>1753</v>

</xml_diff>